<commit_message>
updated results, we now get 85.2% on test
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>method</t>
   </si>
@@ -55,6 +55,9 @@
   </si>
   <si>
     <t>test acc</t>
+  </si>
+  <si>
+    <t>2x200 F G H</t>
   </si>
 </sst>
 </file>
@@ -872,7 +875,7 @@
   <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -946,7 +949,33 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E3" s="1"/>
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3">
+        <v>1E-3</v>
+      </c>
+      <c r="D3">
+        <v>30</v>
+      </c>
+      <c r="E3" s="1">
+        <v>2.9861111111111113E-2</v>
+      </c>
+      <c r="F3" s="5">
+        <v>0.85409500000000005</v>
+      </c>
+      <c r="G3" s="5">
+        <v>0.85148599999999997</v>
+      </c>
+      <c r="H3" s="5">
+        <v>0.85470400000000002</v>
+      </c>
+      <c r="I3" s="5">
+        <v>0.85199499999999995</v>
+      </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E4" s="1"/>

</xml_diff>

<commit_message>
normalize embeddings, not a descernable difference
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
   <si>
     <t>method</t>
   </si>
@@ -58,6 +58,18 @@
   </si>
   <si>
     <t>2x200 F G H</t>
+  </si>
+  <si>
+    <t>norm emb</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>train loss</t>
   </si>
 </sst>
 </file>
@@ -872,158 +884,204 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11" customWidth="1"/>
-    <col min="3" max="3" width="6.7109375" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" customWidth="1"/>
-    <col min="6" max="6" width="8.85546875" style="5" customWidth="1"/>
-    <col min="7" max="7" width="8.5703125" style="5" customWidth="1"/>
-    <col min="8" max="8" width="11.85546875" style="5" customWidth="1"/>
-    <col min="9" max="9" width="20.85546875" style="5" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" customWidth="1"/>
+    <col min="3" max="3" width="11" customWidth="1"/>
+    <col min="4" max="4" width="6.7109375" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" style="5" customWidth="1"/>
+    <col min="8" max="8" width="8.85546875" style="5" customWidth="1"/>
+    <col min="9" max="9" width="8.5703125" style="5" customWidth="1"/>
+    <col min="10" max="10" width="11.85546875" style="5" customWidth="1"/>
+    <col min="11" max="11" width="20.85546875" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
         <v>6</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>1E-3</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>30</v>
       </c>
-      <c r="E2" s="1">
+      <c r="F2" s="1">
         <v>1.9444444444444445E-2</v>
       </c>
-      <c r="F2" s="5">
+      <c r="H2" s="5">
         <v>0.84362899999999996</v>
       </c>
-      <c r="G2" s="5">
+      <c r="I2" s="5">
         <v>0.83591199999999999</v>
       </c>
-      <c r="H2" s="5">
+      <c r="J2" s="5">
         <v>0.84525499999999998</v>
       </c>
-      <c r="I2" s="5">
+      <c r="K2" s="5">
         <v>0.83784599999999998</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
         <v>11</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>1E-3</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>30</v>
       </c>
-      <c r="E3" s="1">
+      <c r="F3" s="1">
         <v>2.9861111111111113E-2</v>
       </c>
-      <c r="F3" s="5">
+      <c r="H3" s="5">
         <v>0.85409500000000005</v>
       </c>
-      <c r="G3" s="5">
+      <c r="I3" s="5">
         <v>0.85148599999999997</v>
       </c>
-      <c r="H3" s="5">
+      <c r="J3" s="5">
         <v>0.85470400000000002</v>
       </c>
-      <c r="I3" s="5">
+      <c r="K3" s="5">
         <v>0.85199499999999995</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E4" s="1"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E5" s="1"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E6" s="1"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E7" s="1"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E8" s="1"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E9" s="1"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E10" s="1"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E11" s="1"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E12" s="1"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E13" s="1"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E14" s="1"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E15" s="1"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E16" s="1"/>
-    </row>
-    <row r="17" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E17" s="1"/>
-    </row>
-    <row r="18" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E18" s="1"/>
-    </row>
-    <row r="19" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E19" s="1"/>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4">
+        <v>1E-3</v>
+      </c>
+      <c r="E4">
+        <v>30</v>
+      </c>
+      <c r="F4" s="1">
+        <v>2.9861111111111113E-2</v>
+      </c>
+      <c r="G4" s="5">
+        <v>0.38289800000000002</v>
+      </c>
+      <c r="H4" s="5">
+        <v>0.854908</v>
+      </c>
+      <c r="I4" s="5">
+        <v>0.85107900000000003</v>
+      </c>
+      <c r="J4" s="5">
+        <v>0.85714299999999999</v>
+      </c>
+      <c r="K4" s="5">
+        <v>0.85097699999999998</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F5" s="1"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F6" s="1"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F7" s="1"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F8" s="1"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F9" s="1"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F10" s="1"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F11" s="1"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F12" s="1"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F13" s="1"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F14" s="1"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F15" s="1"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F16" s="1"/>
+    </row>
+    <row r="17" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F17" s="1"/>
+    </row>
+    <row r="18" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F18" s="1"/>
+    </row>
+    <row r="19" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F19" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>